<commit_message>
porządek - v26 wykresy jasne tło 20.08.2020
</commit_message>
<xml_diff>
--- a/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
+++ b/Sprawozdanie/moje/rysunki/mgr wykresy.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AnnaKułacz\studia\Magisterka\Praca Magisterska\ImmunochemioTherapyModel\Sprawozdanie\moje\rysunki\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDB6C6C-36AD-4FB1-9A56-1A6943201425}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{1DC66E2F-FA51-41BE-990C-40A94CDDCB53}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>T(0)</t>
   </si>
@@ -44,15 +38,52 @@
   <si>
     <t>Promień nowotworu</t>
   </si>
+  <si>
+    <r>
+      <t>x 10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FFBFBFBF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFBFBFBF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FFBFBFBF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -79,13 +110,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -101,48 +135,22 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="32"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Liczba komórek nowotworu T(120) w ostatnim</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> dniu symulacji trwającej</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t> 120 dni</a:t>
+              <a:t>Liczba komórek nowotworu T(120) w ostatnim dniu symulacji trwającej 120 dni</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="pl-PL"/>
@@ -155,40 +163,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
+      <c:layout/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -203,21 +183,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow>
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -299,67 +264,35 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-F0F4-42B0-87D4-0398B203BEA1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="417685728"/>
-        <c:axId val="417685072"/>
+        <c:dLbls/>
+        <c:axId val="76478336"/>
+        <c:axId val="71741824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417685728"/>
+        <c:axId val="76478336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="900000"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" vert="horz"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                <a:pPr algn="ctr">
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200" baseline="0"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Początkowa liczba komórek nowotworowych T(0)</a:t>
                 </a:r>
               </a:p>
@@ -369,413 +302,158 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.313650852160477"/>
+              <c:x val="0.31365085216047706"/>
               <c:y val="0.93318449206635712"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417685072"/>
+        <c:crossAx val="71741824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="tenMillions"/>
           <c:dispUnitsLbl>
+            <c:layout/>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="0" vert="horz"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="75000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
+                    <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000"/>
-                    <a:t>x</a:t>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="en-US" sz="1000"/>
-                    <a:t> 10</a:t>
-                  </a:r>
-                  <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" strike="noStrike" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>7</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US" sz="1000"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:rich>
             </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="417685072"/>
+        <c:axId val="71741824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Liczba komórek nowotworowych po symulacji T(120)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417685728"/>
+        <c:crossAx val="76478336"/>
         <c:crossesAt val="0.5"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:custUnit val="1000000000"/>
           <c:dispUnitsLbl>
+            <c:layout/>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="-5400000" vert="horz"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="75000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
+                    <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>9</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US" sz="1000"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:rich>
             </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="32"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Liczba komórek nowotworu</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> T(120) w ostatnim dniu symulacji trwającej</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t> 120 dni </a:t>
+              <a:t>Liczba komórek nowotworu T(120) w ostatnim dniu symulacji trwającej 120 dni </a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -789,40 +467,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
+      <c:layout/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -837,21 +487,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow>
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -933,66 +568,34 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D6E9-4B21-B813-818C8147ECD2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="590061608"/>
-        <c:axId val="590061936"/>
+        <c:dLbls/>
+        <c:axId val="72025600"/>
+        <c:axId val="72036352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="590061608"/>
+        <c:axId val="72025600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" vert="horz"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                <a:pPr algn="ctr">
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Początkowa Liczba limfocytów krążących C(0)</a:t>
                 </a:r>
               </a:p>
@@ -1002,397 +605,158 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.33246069065034584"/>
-              <c:y val="0.9435994173641884"/>
+              <c:x val="0.33246069065034595"/>
+              <c:y val="0.94359941736418873"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="590061936"/>
+        <c:crossAx val="72036352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:custUnit val="10000000000"/>
           <c:dispUnitsLbl>
+            <c:layout/>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="0" vert="horz"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="75000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
+                    <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>10</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US" sz="1000"/>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:rich>
             </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="590061936"/>
+        <c:axId val="72036352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Liczba komórek nowotworowych po symulacji T(120)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="590061608"/>
+        <c:crossAx val="72025600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:custUnit val="1000000000"/>
           <c:dispUnitsLbl>
+            <c:layout/>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="-5400000" vert="horz"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="75000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
+                    <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>9</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US" sz="1000"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:rich>
             </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="32"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
@@ -1412,44 +776,15 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18228763196779343"/>
-          <c:y val="2.0839144774625468E-2"/>
+          <c:x val="0.18228763196779346"/>
+          <c:y val="2.0839144774625479E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1464,21 +799,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow>
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1561,65 +881,34 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D802-4B78-9EF9-549F9D285B2B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="428872048"/>
-        <c:axId val="428869424"/>
+        <c:dLbls/>
+        <c:axId val="72168576"/>
+        <c:axId val="72170880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="428872048"/>
+        <c:axId val="72168576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" vert="horz"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                <a:pPr algn="ctr">
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Początkowa liczba komórek nowotworowych T(0)</a:t>
                 </a:r>
               </a:p>
@@ -1629,349 +918,136 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.34662294757445899"/>
+              <c:x val="0.34662294757445911"/>
               <c:y val="0.93439484436276521"/>
             </c:manualLayout>
           </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="428869424"/>
+        <c:crossAx val="72170880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:builtInUnit val="tenMillions"/>
           <c:dispUnitsLbl>
+            <c:layout/>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="0" vert="horz"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="75000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
+                    <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>7</a:t>
                   </a:r>
-                  <a:endParaRPr lang="en-US" sz="1000"/>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:rich>
             </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="428869424"/>
+        <c:axId val="72170880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Promień nowotworu po symulacji [mm]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="428872048"/>
+        <c:crossAx val="72168576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:style val="32"/>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="85000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="pl-PL"/>
-              <a:t>Długość promienia nowotworu w ostatnim</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" baseline="0"/>
-              <a:t> dniu symulacji trwającej</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL"/>
-              <a:t> 120 dni</a:t>
+              <a:t>Długość promienia nowotworu w ostatnim dniu symulacji trwającej 120 dni</a:t>
             </a:r>
             <a:br>
               <a:rPr lang="pl-PL"/>
@@ -1983,40 +1059,12 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
+      <c:layout/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2031,21 +1079,6 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow>
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -2128,360 +1161,144 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3124-42FD-A645-ECE2E497A183}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="420572504"/>
-        <c:axId val="420573488"/>
+        <c:dLbls/>
+        <c:axId val="72208768"/>
+        <c:axId val="72211072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="420572504"/>
+        <c:axId val="72208768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" vert="horz"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                <a:pPr algn="ctr">
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Początkowa liczba limfocytów krążących C(0)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420573488"/>
+        <c:crossAx val="72211072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
           <c:custUnit val="10000000000"/>
           <c:dispUnitsLbl>
+            <c:layout/>
             <c:tx>
               <c:rich>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:bodyPr rot="0" vert="horz"/>
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="75000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
+                    <a:defRPr/>
                   </a:pPr>
                   <a:r>
-                    <a:rPr lang="en-US" sz="1000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
                     <a:t>x 10</a:t>
                   </a:r>
                   <a:r>
-                    <a:rPr lang="pl-PL" sz="1000" baseline="30000"/>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="30000"/>
                     <a:t>10</a:t>
                   </a:r>
+                  <a:r>
+                    <a:rPr lang="pl-PL" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0"/>
+                    <a:t> </a:t>
+                  </a:r>
+                  <a:endParaRPr lang="pl-PL"/>
                 </a:p>
               </c:rich>
             </c:tx>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pl-PL"/>
-              </a:p>
-            </c:txPr>
           </c:dispUnitsLbl>
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="420573488"/>
+        <c:axId val="72211072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="-5400000" vert="horz"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
+                  <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="pl-PL" sz="1200"/>
+                  <a:rPr lang="pl-PL" sz="1600"/>
                   <a:t>Promień nowotworu po symulacji [mm]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
-            </a:p>
-          </c:txPr>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-60000000" vert="horz"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="420572504"/>
+        <c:crossAx val="72208768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
-    </a:p>
-  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4803,23 +3620,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>7932</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>15874</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>13608</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>103187</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>128814</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946062AB-FCB7-4EF9-8EF5-55161E9A1F94}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{946062AB-FCB7-4EF9-8EF5-55161E9A1F94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4839,23 +3656,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>136885</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>22585</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>22254</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>222310</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>134154</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F57A29C-35AD-4992-973C-8BCDF75B5F66}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5F57A29C-35AD-4992-973C-8BCDF75B5F66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4875,23 +3692,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>90712</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>14512</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>113845</xdr:rowOff>
+      <xdr:rowOff>190044</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>169334</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>36285</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEF71E4B-E31E-4131-9309-19C91C28E584}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CEF71E4B-E31E-4131-9309-19C91C28E584}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4911,23 +3728,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>215300</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>140727</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>468393</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>186991</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>261724</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>59444</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>462643</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{349718E8-6F30-4F01-891D-DCC2703F7BDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{349718E8-6F30-4F01-891D-DCC2703F7BDB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4991,7 +3808,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5043,7 +3860,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5237,27 +4054,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72E200FD-59F7-4853-9838-C34C44D44042}">
-  <dimension ref="D4:E55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="D4:AN58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+    <sheetView tabSelected="1" topLeftCell="O34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AM31" sqref="AM31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:5">
       <c r="D4" t="s">
         <v>0</v>
       </c>
@@ -5265,7 +4082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="4:5">
       <c r="D5" s="2">
         <v>1000000</v>
       </c>
@@ -5273,7 +4090,7 @@
         <v>6.7599999999999997E-8</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:5">
       <c r="D6" s="2">
         <v>2000000</v>
       </c>
@@ -5281,7 +4098,7 @@
         <v>8.1499999999999995E-8</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="4:5">
       <c r="D7" s="2">
         <v>5000000</v>
       </c>
@@ -5289,7 +4106,7 @@
         <v>2.6899999999999999E-8</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:5">
       <c r="D8" s="2">
         <v>10000000</v>
       </c>
@@ -5297,7 +4114,7 @@
         <v>3.4399999999999997E-8</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:5">
       <c r="D9" s="2">
         <v>15000000</v>
       </c>
@@ -5305,7 +4122,7 @@
         <v>4.4099999999999998E-8</v>
       </c>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:5">
       <c r="D10" s="2">
         <v>17000000</v>
       </c>
@@ -5313,7 +4130,7 @@
         <v>2.96E-8</v>
       </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:5">
       <c r="D11" s="2">
         <v>17500000</v>
       </c>
@@ -5321,7 +4138,7 @@
         <v>3.6699999999999998E-8</v>
       </c>
     </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:5">
       <c r="D12" s="2">
         <v>18000000</v>
       </c>
@@ -5329,7 +4146,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:5">
       <c r="D13" s="2">
         <v>20000000</v>
       </c>
@@ -5337,7 +4154,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="14" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:5">
       <c r="D14" s="2">
         <v>50000000</v>
       </c>
@@ -5345,7 +4162,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:5">
       <c r="D16" t="s">
         <v>2</v>
       </c>
@@ -5353,7 +4170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:5">
       <c r="D17" s="2">
         <v>60000000000</v>
       </c>
@@ -5361,7 +4178,7 @@
         <v>6.7599999999999997E-8</v>
       </c>
     </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:5">
       <c r="D18" s="2">
         <v>30000000000</v>
       </c>
@@ -5369,7 +4186,7 @@
         <v>1.6899999999999999E-7</v>
       </c>
     </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:5">
       <c r="D19" s="2">
         <v>10000000000</v>
       </c>
@@ -5377,7 +4194,7 @@
         <v>3.0899999999999999E-8</v>
       </c>
     </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:5">
       <c r="D20" s="2">
         <v>6000000000</v>
       </c>
@@ -5385,7 +4202,7 @@
         <v>4.7899999999999999E-8</v>
       </c>
     </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:5">
       <c r="D21" s="2">
         <v>4000000000</v>
       </c>
@@ -5393,7 +4210,7 @@
         <v>5.7200000000000003E-8</v>
       </c>
     </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:5">
       <c r="D22" s="2">
         <v>3500000000</v>
       </c>
@@ -5401,7 +4218,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:5">
       <c r="D23" s="2">
         <v>3000000000</v>
       </c>
@@ -5409,7 +4226,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:5">
       <c r="D24" s="2">
         <v>1000000000</v>
       </c>
@@ -5417,7 +4234,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:5">
       <c r="D25" s="2">
         <v>600000000</v>
       </c>
@@ -5425,7 +4242,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:5">
       <c r="D26" s="2">
         <v>300000000</v>
       </c>
@@ -5433,7 +4250,7 @@
         <v>980000000</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5">
       <c r="D33" t="s">
         <v>0</v>
       </c>
@@ -5441,7 +4258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5">
       <c r="D34" s="2">
         <v>1000000</v>
       </c>
@@ -5449,7 +4266,7 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5">
       <c r="D35" s="2">
         <v>2000000</v>
       </c>
@@ -5457,7 +4274,7 @@
         <v>2.6999999999999999E-5</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5">
       <c r="D36" s="2">
         <v>5000000</v>
       </c>
@@ -5465,7 +4282,7 @@
         <v>1.9000000000000001E-5</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5">
       <c r="D37" s="2">
         <v>10000000</v>
       </c>
@@ -5473,7 +4290,7 @@
         <v>2.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5">
       <c r="D38" s="2">
         <v>15000000</v>
       </c>
@@ -5481,7 +4298,7 @@
         <v>2.1999999999999999E-5</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5">
       <c r="D39" s="2">
         <v>17000000</v>
       </c>
@@ -5489,7 +4306,7 @@
         <v>1.9000000000000001E-5</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5">
       <c r="D40" s="2">
         <v>17500000</v>
       </c>
@@ -5497,7 +4314,7 @@
         <v>2.0999999999999999E-5</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5">
       <c r="D41" s="2">
         <v>18000000</v>
       </c>
@@ -5505,7 +4322,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:5">
       <c r="D42" s="2">
         <v>20000000</v>
       </c>
@@ -5513,7 +4330,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5">
       <c r="D43" s="1">
         <v>50000000</v>
       </c>
@@ -5521,7 +4338,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5">
       <c r="D45" t="s">
         <v>2</v>
       </c>
@@ -5529,7 +4346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5">
       <c r="D46" s="2">
         <v>60000000000</v>
       </c>
@@ -5537,7 +4354,7 @@
         <v>2.5000000000000001E-5</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:5">
       <c r="D47" s="2">
         <v>30000000000</v>
       </c>
@@ -5545,7 +4362,7 @@
         <v>3.4E-5</v>
       </c>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:5">
       <c r="D48" s="2">
         <v>10000000000</v>
       </c>
@@ -5553,15 +4370,18 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="49" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:40" ht="15.75">
       <c r="D49" s="2">
         <v>6000000000</v>
       </c>
       <c r="E49" s="2">
         <v>2.3E-5</v>
       </c>
+      <c r="AL49" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:40">
       <c r="D50" s="2">
         <v>4000000000</v>
       </c>
@@ -5569,7 +4389,7 @@
         <v>2.4000000000000001E-5</v>
       </c>
     </row>
-    <row r="51" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:40">
       <c r="D51" s="2">
         <v>3500000000</v>
       </c>
@@ -5577,7 +4397,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="52" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:40">
       <c r="D52" s="2">
         <v>3000000000</v>
       </c>
@@ -5585,7 +4405,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="53" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:40">
       <c r="D53" s="2">
         <v>1000000000</v>
       </c>
@@ -5593,7 +4413,7 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="54" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:40">
       <c r="D54" s="2">
         <v>600000000</v>
       </c>
@@ -5601,16 +4421,22 @@
         <v>6.16</v>
       </c>
     </row>
-    <row r="55" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:40">
       <c r="D55" s="2">
         <v>300000000</v>
       </c>
       <c r="E55" s="2">
         <v>6.16</v>
+      </c>
+    </row>
+    <row r="58" spans="4:40" ht="15.75">
+      <c r="AN58" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>